<commit_message>
export excel batch hal : (penerimaan + kondisi barang)
</commit_message>
<xml_diff>
--- a/public/files/template/inventory/bhp_kondisi.xlsx
+++ b/public/files/template/inventory/bhp_kondisi.xlsx
@@ -99,10 +99,10 @@
     <t>[a.tgl_update]</t>
   </si>
   <si>
-    <t>DAFTAR BARANG  HABIS PAKAI KONDISI BARANG</t>
-  </si>
-  <si>
     <t>[a.batch]</t>
+  </si>
+  <si>
+    <t>DAFTAR BARANG  HABIS PAKAI KONDISI BARANG ( [b.jenisbarang] )</t>
   </si>
 </sst>
 </file>
@@ -228,13 +228,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -252,32 +246,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -584,7 +584,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -599,82 +599,82 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
+      <c r="A1" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="4"/>
+      <c r="D4" s="12"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="4"/>
+      <c r="D5" s="12"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="3" t="s">
+      <c r="A6" s="3"/>
+      <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="6"/>
+      <c r="D6" s="12"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="4"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="3" t="s">
+      <c r="A7" s="3"/>
+      <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="7"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="6"/>
+      <c r="D7" s="5"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="4"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
@@ -689,15 +689,15 @@
       <c r="D10" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="E10" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="12" t="s">
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="I10" s="12" t="s">
+      <c r="I10" s="13" t="s">
         <v>21</v>
       </c>
     </row>
@@ -706,73 +706,73 @@
       <c r="B11" s="18"/>
       <c r="C11" s="16"/>
       <c r="D11" s="18"/>
-      <c r="E11" s="14" t="s">
+      <c r="E11" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="F11" s="14" t="s">
+      <c r="F11" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="G11" s="14" t="s">
+      <c r="G11" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="8">
+      <c r="A12" s="6">
         <v>1</v>
       </c>
-      <c r="B12" s="8">
+      <c r="B12" s="6">
         <v>2</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C12" s="6">
         <v>3</v>
       </c>
-      <c r="D12" s="8">
+      <c r="D12" s="6">
         <v>4</v>
       </c>
-      <c r="E12" s="8">
+      <c r="E12" s="6">
         <v>5</v>
       </c>
-      <c r="F12" s="8">
+      <c r="F12" s="6">
         <v>6</v>
       </c>
-      <c r="G12" s="8">
+      <c r="G12" s="6">
         <v>7</v>
       </c>
-      <c r="H12" s="8">
+      <c r="H12" s="6">
         <v>8</v>
       </c>
-      <c r="I12" s="8">
+      <c r="I12" s="6">
         <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="E13" s="10" t="s">
+      <c r="D13" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="F13" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="G13" s="10" t="s">
+      <c r="G13" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H13" s="10" t="s">
+      <c r="H13" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="I13" s="9" t="s">
+      <c r="I13" s="7" t="s">
         <v>26</v>
       </c>
     </row>
@@ -783,13 +783,13 @@
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="H10:H11"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="C6:D6"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="H10:H11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>